<commit_message>
full list, comments until session 9
</commit_message>
<xml_diff>
--- a/zz Overview.xlsx
+++ b/zz Overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mar84qk\Dropbox\Arbeit\Lehre\Biostatistics 23 WS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmieren\R\biostats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A206E5-40A3-4DB0-B0C7-65231FE2285C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EC6F08-21F0-4FEE-B6C4-BA95A3E91023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="6780" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Session</t>
   </si>
@@ -125,7 +125,34 @@
     <t>no</t>
   </si>
   <si>
-    <t>very dry! Intertwine with R code of w8 / w9?</t>
+    <t>Modeling Relationships</t>
+  </si>
+  <si>
+    <t>Theory session of w9. intertwine with R code?</t>
+  </si>
+  <si>
+    <t>very dry! Intertwine with R code of w9? (Theory of the theory of R session)</t>
+  </si>
+  <si>
+    <t>Statistical Analysis</t>
+  </si>
+  <si>
+    <t>GLM</t>
+  </si>
+  <si>
+    <t>GLM R</t>
+  </si>
+  <si>
+    <t>LMM</t>
+  </si>
+  <si>
+    <t>LMM R</t>
+  </si>
+  <si>
+    <t>Question about report</t>
+  </si>
+  <si>
+    <t>extra session: reproducibility</t>
   </si>
 </sst>
 </file>
@@ -492,18 +519,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +544,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -525,7 +552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -533,7 +560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -544,7 +571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -558,7 +585,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -572,7 +599,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -583,7 +610,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -594,7 +621,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -605,7 +632,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -619,7 +646,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -633,7 +660,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -644,7 +671,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>6</v>
       </c>
@@ -655,7 +682,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -666,7 +693,80 @@
         <v>28</v>
       </c>
       <c r="D14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
         <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>